<commit_message>
Fix the objectId bug in puppeteer
</commit_message>
<xml_diff>
--- a/data/websites-2.xlsx
+++ b/data/websites-2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mahdi\Desktop\Projects\netreach\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mahdi\Desktop\Projects\netreach2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1062" uniqueCount="1059">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1063" uniqueCount="1059">
   <si>
     <t>google.com</t>
   </si>
@@ -3533,7 +3533,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P16" sqref="P16"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4922,7 +4922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>128</v>
       </c>
@@ -4930,7 +4930,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>129</v>
       </c>
@@ -4941,7 +4941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>130</v>
       </c>
@@ -4952,7 +4952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>131</v>
       </c>
@@ -4963,7 +4963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>132</v>
       </c>
@@ -4980,7 +4980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>133</v>
       </c>
@@ -4991,7 +4991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>134</v>
       </c>
@@ -5005,7 +5005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>135</v>
       </c>
@@ -5019,7 +5019,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>136</v>
       </c>
@@ -5030,7 +5030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>137</v>
       </c>
@@ -5041,7 +5041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>138</v>
       </c>
@@ -5052,7 +5052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>139</v>
       </c>
@@ -5060,7 +5060,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>140</v>
       </c>
@@ -5073,8 +5073,11 @@
       <c r="D141" s="1" t="s">
         <v>1008</v>
       </c>
-    </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I141">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>141</v>
       </c>
@@ -5085,7 +5088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>142</v>
       </c>
@@ -5093,7 +5096,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>143</v>
       </c>
@@ -7367,6 +7370,9 @@
       <c r="C352">
         <v>1</v>
       </c>
+      <c r="D352" t="s">
+        <v>417</v>
+      </c>
     </row>
     <row r="353" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A353">
@@ -7544,7 +7550,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="369" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A369">
         <v>368</v>
       </c>
@@ -7558,7 +7564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="370" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A370">
         <v>369</v>
       </c>
@@ -7569,7 +7575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="371" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A371">
         <v>370</v>
       </c>
@@ -7577,7 +7583,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="372" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A372">
         <v>371</v>
       </c>
@@ -7588,7 +7594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="373" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A373">
         <v>372</v>
       </c>
@@ -7599,7 +7605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="374" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A374">
         <v>373</v>
       </c>
@@ -7607,7 +7613,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="375" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A375">
         <v>374</v>
       </c>
@@ -7615,7 +7621,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="376" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A376">
         <v>375</v>
       </c>
@@ -7629,7 +7635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="377" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A377">
         <v>376</v>
       </c>
@@ -7643,7 +7649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="378" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A378">
         <v>377</v>
       </c>
@@ -7657,7 +7663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="379" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A379">
         <v>378</v>
       </c>
@@ -7667,8 +7673,11 @@
       <c r="C379">
         <v>1</v>
       </c>
-    </row>
-    <row r="380" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I379">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="380" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A380">
         <v>379</v>
       </c>
@@ -7682,7 +7691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="381" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A381">
         <v>380</v>
       </c>
@@ -7693,7 +7702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="382" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A382">
         <v>381</v>
       </c>
@@ -7701,7 +7710,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="383" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A383">
         <v>382</v>
       </c>
@@ -7712,7 +7721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="384" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A384">
         <v>383</v>
       </c>
@@ -8101,6 +8110,9 @@
       <c r="C419">
         <v>1</v>
       </c>
+      <c r="F419">
+        <v>1</v>
+      </c>
     </row>
     <row r="420" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A420">
@@ -10014,7 +10026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="593" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="593" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A593">
         <v>592</v>
       </c>
@@ -10022,7 +10034,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="594" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="594" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A594">
         <v>593</v>
       </c>
@@ -10033,7 +10045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="595" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="595" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A595">
         <v>594</v>
       </c>
@@ -10041,7 +10053,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="596" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="596" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A596">
         <v>595</v>
       </c>
@@ -10052,7 +10064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="597" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="597" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A597">
         <v>596</v>
       </c>
@@ -10060,7 +10072,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="598" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="598" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A598">
         <v>597</v>
       </c>
@@ -10068,7 +10080,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="599" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="599" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A599">
         <v>598</v>
       </c>
@@ -10082,7 +10094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="600" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="600" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A600">
         <v>599</v>
       </c>
@@ -10090,7 +10102,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="601" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="601" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A601">
         <v>600</v>
       </c>
@@ -10101,7 +10113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="602" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="602" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A602">
         <v>601</v>
       </c>
@@ -10115,7 +10127,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="603" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="603" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A603">
         <v>602</v>
       </c>
@@ -10126,7 +10138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="604" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="604" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A604">
         <v>603</v>
       </c>
@@ -10137,7 +10149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="605" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="605" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A605">
         <v>604</v>
       </c>
@@ -10148,7 +10160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="606" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="606" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A606">
         <v>605</v>
       </c>
@@ -10159,7 +10171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="607" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="607" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A607">
         <v>606</v>
       </c>
@@ -10169,8 +10181,11 @@
       <c r="C607">
         <v>1</v>
       </c>
-    </row>
-    <row r="608" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I607">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="608" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A608">
         <v>607</v>
       </c>
@@ -10360,7 +10375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="625" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="625" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A625">
         <v>624</v>
       </c>
@@ -10368,7 +10383,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="626" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="626" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A626">
         <v>625</v>
       </c>
@@ -10379,7 +10394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="627" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="627" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A627">
         <v>626</v>
       </c>
@@ -10390,7 +10405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="628" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="628" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A628">
         <v>627</v>
       </c>
@@ -10398,7 +10413,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="629" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="629" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A629">
         <v>628</v>
       </c>
@@ -10409,7 +10424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="630" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="630" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A630">
         <v>629</v>
       </c>
@@ -10420,7 +10435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="631" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="631" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A631">
         <v>630</v>
       </c>
@@ -10431,7 +10446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="632" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="632" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A632">
         <v>631</v>
       </c>
@@ -10442,7 +10457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="633" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="633" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A633">
         <v>632</v>
       </c>
@@ -10456,7 +10471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="634" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="634" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A634">
         <v>633</v>
       </c>
@@ -10467,7 +10482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="635" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="635" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A635">
         <v>634</v>
       </c>
@@ -10477,8 +10492,11 @@
       <c r="C635">
         <v>1</v>
       </c>
-    </row>
-    <row r="636" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I635">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="636" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A636">
         <v>635</v>
       </c>
@@ -10489,7 +10507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="637" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="637" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A637">
         <v>636</v>
       </c>
@@ -10500,7 +10518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="638" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="638" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A638">
         <v>637</v>
       </c>
@@ -10511,7 +10529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="639" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="639" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A639">
         <v>638</v>
       </c>
@@ -10522,7 +10540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="640" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="640" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A640">
         <v>639</v>
       </c>
@@ -10718,7 +10736,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="657" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="657" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A657">
         <v>656</v>
       </c>
@@ -10726,7 +10744,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="658" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="658" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A658">
         <v>657</v>
       </c>
@@ -10737,7 +10755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="659" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="659" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A659">
         <v>658</v>
       </c>
@@ -10748,7 +10766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="660" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="660" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A660">
         <v>659</v>
       </c>
@@ -10758,8 +10776,11 @@
       <c r="C660">
         <v>1</v>
       </c>
-    </row>
-    <row r="661" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H660">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="661" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A661">
         <v>660</v>
       </c>
@@ -10770,7 +10791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="662" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="662" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A662">
         <v>661</v>
       </c>
@@ -10781,7 +10802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="663" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="663" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A663">
         <v>662</v>
       </c>
@@ -10792,7 +10813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="664" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="664" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A664">
         <v>663</v>
       </c>
@@ -10803,7 +10824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="665" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="665" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A665">
         <v>664</v>
       </c>
@@ -10811,7 +10832,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="666" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="666" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A666">
         <v>665</v>
       </c>
@@ -10822,7 +10843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="667" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="667" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A667">
         <v>666</v>
       </c>
@@ -10833,7 +10854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="668" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="668" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A668">
         <v>667</v>
       </c>
@@ -10844,7 +10865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="669" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="669" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A669">
         <v>668</v>
       </c>
@@ -10852,7 +10873,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="670" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="670" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A670">
         <v>669</v>
       </c>
@@ -10863,7 +10884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="671" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="671" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A671">
         <v>670</v>
       </c>
@@ -10874,7 +10895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="672" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="672" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A672">
         <v>671</v>
       </c>
@@ -11774,7 +11795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="753" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="753" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A753">
         <v>752</v>
       </c>
@@ -11785,7 +11806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="754" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="754" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A754">
         <v>753</v>
       </c>
@@ -11796,7 +11817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="755" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="755" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A755">
         <v>754</v>
       </c>
@@ -11807,7 +11828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="756" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="756" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A756">
         <v>755</v>
       </c>
@@ -11821,7 +11842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="757" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="757" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A757">
         <v>756</v>
       </c>
@@ -11831,8 +11852,11 @@
       <c r="C757">
         <v>1</v>
       </c>
-    </row>
-    <row r="758" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H757">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="758" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A758">
         <v>757</v>
       </c>
@@ -11846,7 +11870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="759" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="759" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A759">
         <v>758</v>
       </c>
@@ -11857,7 +11881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="760" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="760" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A760">
         <v>759</v>
       </c>
@@ -11868,7 +11892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="761" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="761" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A761">
         <v>760</v>
       </c>
@@ -11879,7 +11903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="762" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="762" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A762">
         <v>761</v>
       </c>
@@ -11890,7 +11914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="763" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="763" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A763">
         <v>762</v>
       </c>
@@ -11898,7 +11922,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="764" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="764" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A764">
         <v>763</v>
       </c>
@@ -11909,7 +11933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="765" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="765" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A765">
         <v>764</v>
       </c>
@@ -11920,7 +11944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="766" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="766" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A766">
         <v>765</v>
       </c>
@@ -11934,7 +11958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="767" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="767" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A767">
         <v>766</v>
       </c>
@@ -11945,7 +11969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="768" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="768" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A768">
         <v>767</v>
       </c>
@@ -13039,7 +13063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="865" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="865" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A865">
         <v>864</v>
       </c>
@@ -13047,7 +13071,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="866" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="866" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A866">
         <v>865</v>
       </c>
@@ -13061,7 +13085,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="867" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="867" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A867">
         <v>866</v>
       </c>
@@ -13075,7 +13099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="868" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="868" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A868">
         <v>867</v>
       </c>
@@ -13086,7 +13110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="869" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="869" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A869">
         <v>868</v>
       </c>
@@ -13097,7 +13121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="870" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="870" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A870">
         <v>869</v>
       </c>
@@ -13108,7 +13132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="871" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="871" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A871">
         <v>870</v>
       </c>
@@ -13119,7 +13143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="872" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="872" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A872">
         <v>871</v>
       </c>
@@ -13130,7 +13154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="873" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="873" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A873">
         <v>872</v>
       </c>
@@ -13138,7 +13162,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="874" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="874" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A874">
         <v>873</v>
       </c>
@@ -13146,7 +13170,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="875" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="875" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A875">
         <v>874</v>
       </c>
@@ -13154,7 +13178,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="876" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="876" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A876">
         <v>875</v>
       </c>
@@ -13168,7 +13192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="877" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="877" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A877">
         <v>876</v>
       </c>
@@ -13178,8 +13202,11 @@
       <c r="C877">
         <v>1</v>
       </c>
-    </row>
-    <row r="878" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I877">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="878" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A878">
         <v>877</v>
       </c>
@@ -13190,7 +13217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="879" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="879" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A879">
         <v>878</v>
       </c>
@@ -13201,7 +13228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="880" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="880" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A880">
         <v>879</v>
       </c>

</xml_diff>

<commit_message>
Skip some unreachable websites
</commit_message>
<xml_diff>
--- a/data/websites-2.xlsx
+++ b/data/websites-2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1063" uniqueCount="1059">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="1061">
   <si>
     <t>google.com</t>
   </si>
@@ -3110,9 +3110,6 @@
     <t>english.news.cn</t>
   </si>
   <si>
-    <t>zenjido.blog.jp</t>
-  </si>
-  <si>
     <t>xxxxx525.com</t>
   </si>
   <si>
@@ -3201,6 +3198,15 @@
   </si>
   <si>
     <t>static.licdn.com/sc/h/9vghoawmkb5fvzav7oabel24l</t>
+  </si>
+  <si>
+    <t>http://blog.jp/</t>
+  </si>
+  <si>
+    <t>www.3dmgame.com</t>
+  </si>
+  <si>
+    <t>Current timeout not sufficient in Puppeteer, However enough in normal Chrome</t>
   </si>
 </sst>
 </file>
@@ -3532,8 +3538,8 @@
   <dimension ref="A1:N1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+      <pane ySplit="1" topLeftCell="A802" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B829" sqref="B829"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3609,7 +3615,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -3633,6 +3639,12 @@
       <c r="C6">
         <v>1</v>
       </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="N6" t="s">
+        <v>1060</v>
+      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -3672,10 +3684,10 @@
         <v>8</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="E10" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -3741,13 +3753,13 @@
         <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="E16" t="s">
-        <v>1035</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3758,7 +3770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3769,7 +3781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3779,8 +3791,14 @@
       <c r="C19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="N19" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3791,7 +3809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3799,7 +3817,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3807,7 +3825,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3818,7 +3836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3829,7 +3847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3840,7 +3858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3848,7 +3866,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3858,8 +3876,14 @@
       <c r="C27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="N27" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3867,7 +3891,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3878,7 +3902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3886,7 +3910,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3897,7 +3921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -4012,10 +4036,10 @@
         <v>40</v>
       </c>
       <c r="D42" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="E42" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -4078,7 +4102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -4089,7 +4113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -4100,7 +4124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -4108,10 +4132,13 @@
         <v>49</v>
       </c>
       <c r="D51" t="s">
-        <v>1042</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1041</v>
+      </c>
+      <c r="I51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -4119,7 +4146,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -4130,7 +4157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -4138,7 +4165,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -4149,7 +4176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -4157,7 +4184,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -4168,7 +4195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -4176,7 +4203,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -4184,7 +4211,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -4198,7 +4225,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -4208,8 +4235,14 @@
       <c r="C61">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I61">
+        <v>1</v>
+      </c>
+      <c r="N61" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -4217,7 +4250,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -4225,7 +4258,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -4239,7 +4272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -4247,7 +4280,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -4258,7 +4291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -4266,7 +4299,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -4274,7 +4307,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -4285,7 +4318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -4293,10 +4326,10 @@
         <v>68</v>
       </c>
       <c r="D70" t="s">
-        <v>1048</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -4304,7 +4337,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -4314,8 +4347,14 @@
       <c r="C72">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I72">
+        <v>1</v>
+      </c>
+      <c r="N72" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -4323,7 +4362,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -4334,7 +4373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -4342,7 +4381,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -4350,10 +4389,10 @@
         <v>74</v>
       </c>
       <c r="D76" t="s">
-        <v>1049</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -4364,7 +4403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -4375,7 +4414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -4383,7 +4422,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -4512,7 +4551,7 @@
         <v>1</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -4757,7 +4796,7 @@
         <v>111</v>
       </c>
       <c r="D113" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
@@ -5338,7 +5377,7 @@
         <v>163</v>
       </c>
       <c r="D165" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
@@ -5421,7 +5460,7 @@
         <v>170</v>
       </c>
       <c r="D172" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
@@ -5448,7 +5487,7 @@
         <v>173</v>
       </c>
       <c r="D175" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.25">
@@ -5492,7 +5531,7 @@
         <v>177</v>
       </c>
       <c r="D179" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
@@ -5635,7 +5674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>192</v>
       </c>
@@ -5646,7 +5685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>193</v>
       </c>
@@ -5657,7 +5696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>194</v>
       </c>
@@ -5668,7 +5707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>195</v>
       </c>
@@ -5679,7 +5718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>196</v>
       </c>
@@ -5690,7 +5729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>197</v>
       </c>
@@ -5701,7 +5740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>198</v>
       </c>
@@ -5715,7 +5754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>199</v>
       </c>
@@ -5726,7 +5765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>200</v>
       </c>
@@ -5734,7 +5773,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>201</v>
       </c>
@@ -5742,7 +5781,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>202</v>
       </c>
@@ -5750,7 +5789,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>203</v>
       </c>
@@ -5761,7 +5800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>204</v>
       </c>
@@ -5772,7 +5811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>205</v>
       </c>
@@ -5782,8 +5821,14 @@
       <c r="C206">
         <v>1</v>
       </c>
-    </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I206">
+        <v>1</v>
+      </c>
+      <c r="N206" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="207" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>206</v>
       </c>
@@ -5797,7 +5842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>207</v>
       </c>
@@ -5805,10 +5850,10 @@
         <v>206</v>
       </c>
       <c r="D208" t="s">
-        <v>1056</v>
-      </c>
-    </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="209" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>208</v>
       </c>
@@ -5819,7 +5864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>209</v>
       </c>
@@ -5830,7 +5875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>210</v>
       </c>
@@ -5840,8 +5885,14 @@
       <c r="C211">
         <v>1</v>
       </c>
-    </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I211">
+        <v>1</v>
+      </c>
+      <c r="N211" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="212" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>211</v>
       </c>
@@ -5852,7 +5903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>212</v>
       </c>
@@ -5860,7 +5911,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>213</v>
       </c>
@@ -5870,8 +5921,14 @@
       <c r="C214">
         <v>1</v>
       </c>
-    </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I214">
+        <v>1</v>
+      </c>
+      <c r="N214" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="215" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>214</v>
       </c>
@@ -5879,10 +5936,10 @@
         <v>213</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>1036</v>
-      </c>
-    </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="216" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>215</v>
       </c>
@@ -5893,7 +5950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>216</v>
       </c>
@@ -5901,7 +5958,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>217</v>
       </c>
@@ -5912,7 +5969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>218</v>
       </c>
@@ -5923,7 +5980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>219</v>
       </c>
@@ -5931,7 +5988,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>220</v>
       </c>
@@ -5939,7 +5996,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>221</v>
       </c>
@@ -5950,7 +6007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>222</v>
       </c>
@@ -5961,7 +6018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>223</v>
       </c>
@@ -6057,7 +6114,7 @@
         <v>230</v>
       </c>
       <c r="D232" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="233" spans="1:9" x14ac:dyDescent="0.25">
@@ -6440,7 +6497,7 @@
         <v>1</v>
       </c>
       <c r="D266" s="1" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="267" spans="1:7" x14ac:dyDescent="0.25">
@@ -6676,10 +6733,10 @@
         <v>286</v>
       </c>
       <c r="D288" s="1" t="s">
-        <v>1052</v>
-      </c>
-    </row>
-    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="289" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>288</v>
       </c>
@@ -6690,7 +6747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>289</v>
       </c>
@@ -6701,7 +6758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>290</v>
       </c>
@@ -6715,7 +6772,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>291</v>
       </c>
@@ -6726,7 +6783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>292</v>
       </c>
@@ -6737,7 +6794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="294" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>293</v>
       </c>
@@ -6748,7 +6805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>294</v>
       </c>
@@ -6759,7 +6816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>295</v>
       </c>
@@ -6767,7 +6824,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A297">
         <v>296</v>
       </c>
@@ -6778,7 +6835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>297</v>
       </c>
@@ -6786,7 +6843,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>298</v>
       </c>
@@ -6797,7 +6854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="300" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>299</v>
       </c>
@@ -6807,8 +6864,14 @@
       <c r="C300">
         <v>1</v>
       </c>
-    </row>
-    <row r="301" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I300">
+        <v>1</v>
+      </c>
+      <c r="N300" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="301" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>300</v>
       </c>
@@ -6819,7 +6882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="302" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>301</v>
       </c>
@@ -6827,7 +6890,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="303" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>302</v>
       </c>
@@ -6838,7 +6901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="304" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>303</v>
       </c>
@@ -7022,6 +7085,9 @@
       <c r="C322">
         <v>1</v>
       </c>
+      <c r="D322" t="s">
+        <v>1059</v>
+      </c>
     </row>
     <row r="323" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A323">
@@ -7186,7 +7252,7 @@
         <v>1017</v>
       </c>
     </row>
-    <row r="337" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A337">
         <v>336</v>
       </c>
@@ -7197,7 +7263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="338" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A338">
         <v>337</v>
       </c>
@@ -7208,7 +7274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="339" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A339">
         <v>338</v>
       </c>
@@ -7219,7 +7285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="340" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A340">
         <v>339</v>
       </c>
@@ -7227,7 +7293,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="341" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A341">
         <v>340</v>
       </c>
@@ -7238,7 +7304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="342" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A342">
         <v>341</v>
       </c>
@@ -7249,7 +7315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="343" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A343">
         <v>342</v>
       </c>
@@ -7263,7 +7329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="344" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A344">
         <v>343</v>
       </c>
@@ -7274,7 +7340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="345" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A345">
         <v>344</v>
       </c>
@@ -7284,8 +7350,14 @@
       <c r="C345">
         <v>1</v>
       </c>
-    </row>
-    <row r="346" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I345">
+        <v>1</v>
+      </c>
+      <c r="N345" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="346" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A346">
         <v>345</v>
       </c>
@@ -7299,7 +7371,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="347" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A347">
         <v>346</v>
       </c>
@@ -7313,7 +7385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="348" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A348">
         <v>347</v>
       </c>
@@ -7324,7 +7396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="349" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A349">
         <v>348</v>
       </c>
@@ -7335,7 +7407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="350" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A350">
         <v>349</v>
       </c>
@@ -7349,7 +7421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="351" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A351">
         <v>350</v>
       </c>
@@ -7360,7 +7432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="352" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A352">
         <v>351</v>
       </c>
@@ -7799,6 +7871,12 @@
       <c r="C391">
         <v>1</v>
       </c>
+      <c r="I391">
+        <v>1</v>
+      </c>
+      <c r="N391" t="s">
+        <v>1060</v>
+      </c>
     </row>
     <row r="392" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A392">
@@ -7902,7 +7980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="401" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A401">
         <v>400</v>
       </c>
@@ -7916,7 +7994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="402" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A402">
         <v>401</v>
       </c>
@@ -7927,7 +8005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="403" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A403">
         <v>402</v>
       </c>
@@ -7938,7 +8016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="404" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A404">
         <v>403</v>
       </c>
@@ -7948,8 +8026,14 @@
       <c r="C404">
         <v>1</v>
       </c>
-    </row>
-    <row r="405" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I404">
+        <v>1</v>
+      </c>
+      <c r="N404" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="405" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A405">
         <v>404</v>
       </c>
@@ -7960,7 +8044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="406" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A406">
         <v>405</v>
       </c>
@@ -7971,7 +8055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="407" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A407">
         <v>406</v>
       </c>
@@ -7982,7 +8066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="408" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A408">
         <v>407</v>
       </c>
@@ -7993,7 +8077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="409" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A409">
         <v>408</v>
       </c>
@@ -8001,7 +8085,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="410" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A410">
         <v>409</v>
       </c>
@@ -8012,7 +8096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="411" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A411">
         <v>410</v>
       </c>
@@ -8023,7 +8107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="412" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A412">
         <v>411</v>
       </c>
@@ -8037,7 +8121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="413" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A413">
         <v>412</v>
       </c>
@@ -8048,7 +8132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="414" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A414">
         <v>413</v>
       </c>
@@ -8056,7 +8140,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="415" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A415">
         <v>414</v>
       </c>
@@ -8070,7 +8154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="416" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A416">
         <v>415</v>
       </c>
@@ -8450,7 +8534,7 @@
         <v>447</v>
       </c>
       <c r="D449" s="1" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="450" spans="1:9" x14ac:dyDescent="0.25">
@@ -8508,7 +8592,7 @@
         <v>452</v>
       </c>
       <c r="D454" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="455" spans="1:9" x14ac:dyDescent="0.25">
@@ -8615,7 +8699,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="465" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A465">
         <v>464</v>
       </c>
@@ -8626,7 +8710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="466" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A466">
         <v>465</v>
       </c>
@@ -8634,7 +8718,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="467" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A467">
         <v>466</v>
       </c>
@@ -8645,7 +8729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="468" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A468">
         <v>467</v>
       </c>
@@ -8656,7 +8740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="469" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A469">
         <v>468</v>
       </c>
@@ -8667,7 +8751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="470" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A470">
         <v>469</v>
       </c>
@@ -8680,8 +8764,14 @@
       <c r="D470" s="1" t="s">
         <v>1020</v>
       </c>
-    </row>
-    <row r="471" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I470">
+        <v>1</v>
+      </c>
+      <c r="N470" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="471" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A471">
         <v>470</v>
       </c>
@@ -8692,7 +8782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="472" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A472">
         <v>471</v>
       </c>
@@ -8703,7 +8793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="473" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A473">
         <v>472</v>
       </c>
@@ -8714,7 +8804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="474" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A474">
         <v>473</v>
       </c>
@@ -8728,7 +8818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="475" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A475">
         <v>474</v>
       </c>
@@ -8739,7 +8829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="476" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A476">
         <v>475</v>
       </c>
@@ -8750,7 +8840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="477" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A477">
         <v>476</v>
       </c>
@@ -8764,7 +8854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="478" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A478">
         <v>477</v>
       </c>
@@ -8775,7 +8865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="479" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A479">
         <v>478</v>
       </c>
@@ -8786,7 +8876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="480" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A480">
         <v>479</v>
       </c>
@@ -8976,6 +9066,9 @@
       <c r="C495">
         <v>1</v>
       </c>
+      <c r="H495">
+        <v>1</v>
+      </c>
     </row>
     <row r="496" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A496">
@@ -8985,7 +9078,7 @@
         <v>494</v>
       </c>
       <c r="D496" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="497" spans="1:3" x14ac:dyDescent="0.25">
@@ -9680,7 +9773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="561" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="561" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A561">
         <v>560</v>
       </c>
@@ -9691,7 +9784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="562" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="562" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A562">
         <v>561</v>
       </c>
@@ -9702,7 +9795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="563" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="563" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A563">
         <v>562</v>
       </c>
@@ -9710,7 +9803,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="564" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="564" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A564">
         <v>563</v>
       </c>
@@ -9721,7 +9814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="565" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="565" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A565">
         <v>564</v>
       </c>
@@ -9731,8 +9824,14 @@
       <c r="C565">
         <v>1</v>
       </c>
-    </row>
-    <row r="566" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I565">
+        <v>1</v>
+      </c>
+      <c r="N565" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="566" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A566">
         <v>565</v>
       </c>
@@ -9740,7 +9839,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="567" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="567" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A567">
         <v>566</v>
       </c>
@@ -9751,7 +9850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="568" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="568" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A568">
         <v>567</v>
       </c>
@@ -9762,7 +9861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="569" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="569" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A569">
         <v>568</v>
       </c>
@@ -9770,7 +9869,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="570" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="570" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A570">
         <v>569</v>
       </c>
@@ -9781,7 +9880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="571" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="571" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A571">
         <v>570</v>
       </c>
@@ -9792,7 +9891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="572" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="572" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A572">
         <v>571</v>
       </c>
@@ -9806,7 +9905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="573" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="573" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A573">
         <v>572</v>
       </c>
@@ -9820,7 +9919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="574" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="574" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A574">
         <v>573</v>
       </c>
@@ -9830,8 +9929,14 @@
       <c r="C574">
         <v>1</v>
       </c>
-    </row>
-    <row r="575" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I574">
+        <v>1</v>
+      </c>
+      <c r="N574" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="575" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A575">
         <v>574</v>
       </c>
@@ -9842,7 +9947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="576" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="576" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A576">
         <v>575</v>
       </c>
@@ -10277,6 +10382,9 @@
       <c r="C616">
         <v>1</v>
       </c>
+      <c r="I616">
+        <v>1</v>
+      </c>
     </row>
     <row r="617" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A617">
@@ -10548,7 +10656,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="641" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="641" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A641">
         <v>640</v>
       </c>
@@ -10559,7 +10667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="642" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="642" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A642">
         <v>641</v>
       </c>
@@ -10573,7 +10681,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="643" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="643" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A643">
         <v>642</v>
       </c>
@@ -10583,8 +10691,11 @@
       <c r="C643">
         <v>1</v>
       </c>
-    </row>
-    <row r="644" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I643">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="644" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A644">
         <v>643</v>
       </c>
@@ -10598,7 +10709,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="645" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="645" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A645">
         <v>644</v>
       </c>
@@ -10609,7 +10720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="646" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="646" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A646">
         <v>645</v>
       </c>
@@ -10617,7 +10728,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="647" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="647" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A647">
         <v>646</v>
       </c>
@@ -10628,7 +10739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="648" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="648" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A648">
         <v>647</v>
       </c>
@@ -10636,7 +10747,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="649" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="649" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A649">
         <v>648</v>
       </c>
@@ -10644,7 +10755,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="650" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="650" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A650">
         <v>649</v>
       </c>
@@ -10655,7 +10766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="651" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="651" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A651">
         <v>650</v>
       </c>
@@ -10669,7 +10780,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="652" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="652" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A652">
         <v>651</v>
       </c>
@@ -10683,7 +10794,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="653" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="653" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A653">
         <v>652</v>
       </c>
@@ -10694,7 +10805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="654" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="654" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A654">
         <v>653</v>
       </c>
@@ -10708,7 +10819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="655" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="655" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A655">
         <v>654</v>
       </c>
@@ -10722,7 +10833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="656" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="656" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A656">
         <v>655</v>
       </c>
@@ -10736,7 +10847,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="657" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="657" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A657">
         <v>656</v>
       </c>
@@ -10744,7 +10855,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="658" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="658" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A658">
         <v>657</v>
       </c>
@@ -10755,7 +10866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="659" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="659" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A659">
         <v>658</v>
       </c>
@@ -10766,7 +10877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="660" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="660" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A660">
         <v>659</v>
       </c>
@@ -10780,7 +10891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="661" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="661" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A661">
         <v>660</v>
       </c>
@@ -10791,7 +10902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="662" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="662" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A662">
         <v>661</v>
       </c>
@@ -10802,7 +10913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="663" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="663" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A663">
         <v>662</v>
       </c>
@@ -10813,7 +10924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="664" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="664" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A664">
         <v>663</v>
       </c>
@@ -10823,8 +10934,11 @@
       <c r="C664">
         <v>1</v>
       </c>
-    </row>
-    <row r="665" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I664">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="665" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A665">
         <v>664</v>
       </c>
@@ -10832,7 +10946,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="666" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="666" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A666">
         <v>665</v>
       </c>
@@ -10843,7 +10957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="667" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="667" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A667">
         <v>666</v>
       </c>
@@ -10854,7 +10968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="668" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="668" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A668">
         <v>667</v>
       </c>
@@ -10865,7 +10979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="669" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="669" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A669">
         <v>668</v>
       </c>
@@ -10873,7 +10987,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="670" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="670" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A670">
         <v>669</v>
       </c>
@@ -10884,7 +10998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="671" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="671" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A671">
         <v>670</v>
       </c>
@@ -10895,7 +11009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="672" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="672" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A672">
         <v>671</v>
       </c>
@@ -10903,7 +11017,7 @@
         <v>670</v>
       </c>
       <c r="D672" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="673" spans="1:7" x14ac:dyDescent="0.25">
@@ -10936,7 +11050,7 @@
         <v>673</v>
       </c>
       <c r="D675" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="676" spans="1:7" x14ac:dyDescent="0.25">
@@ -11781,7 +11895,7 @@
         <v>1</v>
       </c>
       <c r="D751" s="1" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="752" spans="1:9" x14ac:dyDescent="0.25">
@@ -12338,7 +12452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="801" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="801" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A801">
         <v>800</v>
       </c>
@@ -12349,7 +12463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="802" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="802" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A802">
         <v>801</v>
       </c>
@@ -12363,7 +12477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="803" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="803" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A803">
         <v>802</v>
       </c>
@@ -12373,8 +12487,14 @@
       <c r="C803">
         <v>1</v>
       </c>
-    </row>
-    <row r="804" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I803">
+        <v>1</v>
+      </c>
+      <c r="N803" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="804" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A804">
         <v>803</v>
       </c>
@@ -12385,7 +12505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="805" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="805" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A805">
         <v>804</v>
       </c>
@@ -12393,7 +12513,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="806" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="806" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A806">
         <v>805</v>
       </c>
@@ -12404,7 +12524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="807" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="807" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A807">
         <v>806</v>
       </c>
@@ -12415,7 +12535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="808" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="808" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A808">
         <v>807</v>
       </c>
@@ -12426,7 +12546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="809" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="809" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A809">
         <v>808</v>
       </c>
@@ -12437,7 +12557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="810" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="810" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A810">
         <v>809</v>
       </c>
@@ -12445,7 +12565,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="811" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="811" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A811">
         <v>810</v>
       </c>
@@ -12453,7 +12573,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="812" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="812" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A812">
         <v>811</v>
       </c>
@@ -12467,7 +12587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="813" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="813" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A813">
         <v>812</v>
       </c>
@@ -12478,7 +12598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="814" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="814" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A814">
         <v>813</v>
       </c>
@@ -12489,7 +12609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="815" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="815" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A815">
         <v>814</v>
       </c>
@@ -12503,7 +12623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="816" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="816" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A816">
         <v>815</v>
       </c>
@@ -12517,7 +12637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="817" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="817" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A817">
         <v>816</v>
       </c>
@@ -12528,7 +12648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="818" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="818" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A818">
         <v>817</v>
       </c>
@@ -12542,7 +12662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="819" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="819" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A819">
         <v>818</v>
       </c>
@@ -12553,7 +12673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="820" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="820" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A820">
         <v>819</v>
       </c>
@@ -12564,7 +12684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="821" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="821" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A821">
         <v>820</v>
       </c>
@@ -12575,7 +12695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="822" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="822" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A822">
         <v>821</v>
       </c>
@@ -12589,7 +12709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="823" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="823" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A823">
         <v>822</v>
       </c>
@@ -12597,7 +12717,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="824" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="824" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A824">
         <v>823</v>
       </c>
@@ -12608,7 +12728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="825" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="825" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A825">
         <v>824</v>
       </c>
@@ -12619,7 +12739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="826" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="826" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A826">
         <v>825</v>
       </c>
@@ -12633,7 +12753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="827" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="827" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A827">
         <v>826</v>
       </c>
@@ -12644,7 +12764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="828" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="828" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A828">
         <v>827</v>
       </c>
@@ -12658,7 +12778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="829" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="829" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A829">
         <v>828</v>
       </c>
@@ -12668,8 +12788,14 @@
       <c r="C829">
         <v>1</v>
       </c>
-    </row>
-    <row r="830" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I829">
+        <v>1</v>
+      </c>
+      <c r="N829" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="830" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A830">
         <v>829</v>
       </c>
@@ -12680,7 +12806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="831" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="831" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A831">
         <v>830</v>
       </c>
@@ -12691,7 +12817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="832" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="832" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A832">
         <v>831</v>
       </c>
@@ -12702,7 +12828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="833" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="833" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A833">
         <v>832</v>
       </c>
@@ -12710,10 +12836,10 @@
         <v>831</v>
       </c>
       <c r="D833" t="s">
-        <v>1058</v>
-      </c>
-    </row>
-    <row r="834" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="834" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A834">
         <v>833</v>
       </c>
@@ -12724,7 +12850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="835" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="835" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A835">
         <v>834</v>
       </c>
@@ -12734,8 +12860,14 @@
       <c r="C835">
         <v>1</v>
       </c>
-    </row>
-    <row r="836" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I835">
+        <v>1</v>
+      </c>
+      <c r="N835" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="836" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A836">
         <v>835</v>
       </c>
@@ -12746,7 +12878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="837" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="837" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A837">
         <v>836</v>
       </c>
@@ -12757,7 +12889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="838" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="838" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A838">
         <v>837</v>
       </c>
@@ -12771,7 +12903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="839" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="839" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A839">
         <v>838</v>
       </c>
@@ -12782,7 +12914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="840" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="840" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A840">
         <v>839</v>
       </c>
@@ -12793,7 +12925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="841" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="841" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A841">
         <v>840</v>
       </c>
@@ -12804,7 +12936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="842" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="842" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A842">
         <v>841</v>
       </c>
@@ -12815,7 +12947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="843" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="843" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A843">
         <v>842</v>
       </c>
@@ -12823,7 +12955,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="844" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="844" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A844">
         <v>843</v>
       </c>
@@ -12834,7 +12966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="845" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="845" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A845">
         <v>844</v>
       </c>
@@ -12845,7 +12977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="846" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="846" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A846">
         <v>845</v>
       </c>
@@ -12856,7 +12988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="847" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="847" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A847">
         <v>846</v>
       </c>
@@ -12867,7 +12999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="848" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="848" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A848">
         <v>847</v>
       </c>
@@ -13081,8 +13213,8 @@
       <c r="C866">
         <v>1</v>
       </c>
-      <c r="D866" t="s">
-        <v>1028</v>
+      <c r="D866" s="1" t="s">
+        <v>1058</v>
       </c>
     </row>
     <row r="867" spans="1:9" x14ac:dyDescent="0.25">
@@ -13452,7 +13584,7 @@
         <v>1</v>
       </c>
       <c r="D898" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="899" spans="1:9" x14ac:dyDescent="0.25">
@@ -14096,7 +14228,7 @@
         <v>1</v>
       </c>
       <c r="D956" s="1" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="957" spans="1:7" x14ac:dyDescent="0.25">
@@ -14242,7 +14374,7 @@
         <v>1</v>
       </c>
       <c r="D969" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="970" spans="1:7" x14ac:dyDescent="0.25">
@@ -14399,7 +14531,7 @@
         <v>981</v>
       </c>
       <c r="D983" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="984" spans="1:7" x14ac:dyDescent="0.25">
@@ -14620,8 +14752,9 @@
     <hyperlink ref="D4" r:id="rId15" display="https://code.visualstudio.com/assets/docs/cpp/playbutton/run-play-button.png"/>
     <hyperlink ref="D449" r:id="rId16" display="https://i.pinimg.com/originals/cc/c0/8c/ccc08caae32587d82de28de9cd96abf5.jpg"/>
     <hyperlink ref="D288" r:id="rId17"/>
+    <hyperlink ref="D866" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId18"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId19"/>
 </worksheet>
 </file>
</xml_diff>